<commit_message>
created functions to store info from excell sheet in objects and create an invoice based on those objects
</commit_message>
<xml_diff>
--- a/src/python/Excell_exercise/Invoices.xlsx
+++ b/src/python/Excell_exercise/Invoices.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Customer" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>ID</t>
   </si>
@@ -426,7 +426,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -511,8 +511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,10 +594,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,223 +607,283 @@
     <col min="3" max="3" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>3</v>
       </c>
       <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C11">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B12">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C12">
+        <v>5</v>
+      </c>
+      <c r="D12">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C14">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="B16">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C16">
+        <v>5</v>
+      </c>
+      <c r="D16">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B17">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="B18">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C18">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="B19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added more data to invoices spreadsheet
</commit_message>
<xml_diff>
--- a/src/python/Excell_exercise/Invoices.xlsx
+++ b/src/python/Excell_exercise/Invoices.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Customer" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
   <si>
     <t>ID</t>
   </si>
@@ -102,6 +102,48 @@
   </si>
   <si>
     <t>Jessica</t>
+  </si>
+  <si>
+    <t>Jerry</t>
+  </si>
+  <si>
+    <t>Foster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kay </t>
+  </si>
+  <si>
+    <t>Ellison</t>
+  </si>
+  <si>
+    <t>TJ</t>
+  </si>
+  <si>
+    <t>Whitworth</t>
+  </si>
+  <si>
+    <t>Mikhail</t>
+  </si>
+  <si>
+    <t>Proctor</t>
+  </si>
+  <si>
+    <t>Sylvie</t>
+  </si>
+  <si>
+    <t>Mcfadden</t>
+  </si>
+  <si>
+    <t>Renesmae</t>
+  </si>
+  <si>
+    <t>Werner</t>
+  </si>
+  <si>
+    <t>Laurvn</t>
+  </si>
+  <si>
+    <t>Green</t>
   </si>
 </sst>
 </file>
@@ -424,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,6 +544,83 @@
         <v>23</v>
       </c>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -509,10 +628,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,7 +656,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>43811</v>
+        <v>43800</v>
       </c>
       <c r="C2">
         <v>3</v>
@@ -548,7 +667,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>43829</v>
+        <v>43800</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -559,7 +678,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>43832</v>
+        <v>43801</v>
       </c>
       <c r="C4">
         <v>4</v>
@@ -570,7 +689,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>43846</v>
+        <v>43802</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -581,10 +700,373 @@
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>43856</v>
+        <v>43803</v>
       </c>
       <c r="C6">
         <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>43803</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
+        <v>43804</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2">
+        <v>43804</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2">
+        <v>43805</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2">
+        <v>43806</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2">
+        <v>43807</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2">
+        <v>43808</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2">
+        <v>43809</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2">
+        <v>43810</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2">
+        <v>43811</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2">
+        <v>43812</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2">
+        <v>43813</v>
+      </c>
+      <c r="C18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2">
+        <v>43814</v>
+      </c>
+      <c r="C19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2">
+        <v>43815</v>
+      </c>
+      <c r="C20">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2">
+        <v>43816</v>
+      </c>
+      <c r="C21">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2">
+        <v>43817</v>
+      </c>
+      <c r="C22">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2">
+        <v>43817</v>
+      </c>
+      <c r="C23">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2">
+        <v>44184</v>
+      </c>
+      <c r="C24">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2">
+        <v>43819</v>
+      </c>
+      <c r="C25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2">
+        <v>43820</v>
+      </c>
+      <c r="C26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" s="2">
+        <v>43820</v>
+      </c>
+      <c r="C27">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" s="2">
+        <v>43821</v>
+      </c>
+      <c r="C28">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2">
+        <v>43822</v>
+      </c>
+      <c r="C29">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" s="2">
+        <v>43823</v>
+      </c>
+      <c r="C30">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" s="2">
+        <v>43824</v>
+      </c>
+      <c r="C31">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" s="2">
+        <v>43825</v>
+      </c>
+      <c r="C32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" s="2">
+        <v>43826</v>
+      </c>
+      <c r="C33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" s="2">
+        <v>43826</v>
+      </c>
+      <c r="C34">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" s="2">
+        <v>43827</v>
+      </c>
+      <c r="C35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" s="2">
+        <v>43828</v>
+      </c>
+      <c r="C36">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" s="2">
+        <v>43828</v>
+      </c>
+      <c r="C37">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" s="2">
+        <v>43829</v>
+      </c>
+      <c r="C38">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" s="2">
+        <v>43830</v>
+      </c>
+      <c r="C39">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -594,10 +1076,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D151"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="H139" sqref="H139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,7 +1108,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>4</v>
@@ -640,7 +1122,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>3</v>
@@ -654,7 +1136,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -668,7 +1150,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -682,7 +1164,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -696,7 +1178,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -710,7 +1192,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8">
         <v>4</v>
@@ -724,7 +1206,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9">
         <v>3</v>
@@ -738,7 +1220,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -766,7 +1248,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C12">
         <v>5</v>
@@ -780,7 +1262,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C13">
         <v>4</v>
@@ -794,7 +1276,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C14">
         <v>3</v>
@@ -808,7 +1290,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C15">
         <v>2</v>
@@ -822,7 +1304,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C16">
         <v>5</v>
@@ -836,7 +1318,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C17">
         <v>4</v>
@@ -850,7 +1332,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C18">
         <v>3</v>
@@ -864,7 +1346,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -878,13 +1360,1847 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20">
         <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>5</v>
+      </c>
+      <c r="C21">
+        <v>5</v>
+      </c>
+      <c r="D21">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>5</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>6</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>6</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>6</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>7</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>7</v>
+      </c>
+      <c r="C27">
+        <v>5</v>
+      </c>
+      <c r="D27">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>7</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>7</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>8</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>8</v>
+      </c>
+      <c r="C31">
+        <v>5</v>
+      </c>
+      <c r="D31">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>8</v>
+      </c>
+      <c r="C32">
+        <v>4</v>
+      </c>
+      <c r="D32">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>8</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>9</v>
+      </c>
+      <c r="C34">
+        <v>5</v>
+      </c>
+      <c r="D34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>9</v>
+      </c>
+      <c r="C35">
+        <v>4</v>
+      </c>
+      <c r="D35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>9</v>
+      </c>
+      <c r="C36">
+        <v>3</v>
+      </c>
+      <c r="D36">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>10</v>
+      </c>
+      <c r="C37">
+        <v>3</v>
+      </c>
+      <c r="D37">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>10</v>
+      </c>
+      <c r="C38">
+        <v>2</v>
+      </c>
+      <c r="D38">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>10</v>
+      </c>
+      <c r="C39">
+        <v>2</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>10</v>
+      </c>
+      <c r="C40">
+        <v>2</v>
+      </c>
+      <c r="D40">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>11</v>
+      </c>
+      <c r="C41">
+        <v>4</v>
+      </c>
+      <c r="D41">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>11</v>
+      </c>
+      <c r="C42">
+        <v>2</v>
+      </c>
+      <c r="D42">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>11</v>
+      </c>
+      <c r="C43">
+        <v>3</v>
+      </c>
+      <c r="D43">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>12</v>
+      </c>
+      <c r="C44">
+        <v>3</v>
+      </c>
+      <c r="D44">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <v>12</v>
+      </c>
+      <c r="C45">
+        <v>2</v>
+      </c>
+      <c r="D45">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <v>12</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <v>13</v>
+      </c>
+      <c r="C47">
+        <v>2</v>
+      </c>
+      <c r="D47">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>13</v>
+      </c>
+      <c r="C48">
+        <v>5</v>
+      </c>
+      <c r="D48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <v>13</v>
+      </c>
+      <c r="C49">
+        <v>5</v>
+      </c>
+      <c r="D49">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <v>13</v>
+      </c>
+      <c r="C50">
+        <v>4</v>
+      </c>
+      <c r="D50">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>13</v>
+      </c>
+      <c r="C51">
+        <v>4</v>
+      </c>
+      <c r="D51">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <v>14</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <v>14</v>
+      </c>
+      <c r="C53">
+        <v>2</v>
+      </c>
+      <c r="D53">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54">
+        <v>14</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55">
+        <v>14</v>
+      </c>
+      <c r="C55">
+        <v>4</v>
+      </c>
+      <c r="D55">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56">
+        <v>15</v>
+      </c>
+      <c r="C56">
+        <v>2</v>
+      </c>
+      <c r="D56">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57">
+        <v>15</v>
+      </c>
+      <c r="C57">
+        <v>2</v>
+      </c>
+      <c r="D57">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58">
+        <v>15</v>
+      </c>
+      <c r="C58">
+        <v>5</v>
+      </c>
+      <c r="D58">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59">
+        <v>16</v>
+      </c>
+      <c r="C59">
+        <v>2</v>
+      </c>
+      <c r="D59">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60">
+        <v>16</v>
+      </c>
+      <c r="C60">
+        <v>4</v>
+      </c>
+      <c r="D60">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61">
+        <v>16</v>
+      </c>
+      <c r="C61">
+        <v>3</v>
+      </c>
+      <c r="D61">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62">
+        <v>16</v>
+      </c>
+      <c r="C62">
+        <v>3</v>
+      </c>
+      <c r="D62">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63">
+        <v>17</v>
+      </c>
+      <c r="C63">
+        <v>2</v>
+      </c>
+      <c r="D63">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64">
+        <v>17</v>
+      </c>
+      <c r="C64">
+        <v>4</v>
+      </c>
+      <c r="D64">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65">
+        <v>17</v>
+      </c>
+      <c r="C65">
+        <v>5</v>
+      </c>
+      <c r="D65">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66">
+        <v>18</v>
+      </c>
+      <c r="C66">
+        <v>5</v>
+      </c>
+      <c r="D66">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67">
+        <v>18</v>
+      </c>
+      <c r="C67">
+        <v>5</v>
+      </c>
+      <c r="D67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68">
+        <v>18</v>
+      </c>
+      <c r="C68">
+        <v>4</v>
+      </c>
+      <c r="D68">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69">
+        <v>18</v>
+      </c>
+      <c r="C69">
+        <v>5</v>
+      </c>
+      <c r="D69">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70">
+        <v>19</v>
+      </c>
+      <c r="C70">
+        <v>3</v>
+      </c>
+      <c r="D70">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71">
+        <v>19</v>
+      </c>
+      <c r="C71">
+        <v>4</v>
+      </c>
+      <c r="D71">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72">
+        <v>19</v>
+      </c>
+      <c r="C72">
+        <v>4</v>
+      </c>
+      <c r="D72">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73">
+        <v>19</v>
+      </c>
+      <c r="C73">
+        <v>5</v>
+      </c>
+      <c r="D73">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74">
+        <v>19</v>
+      </c>
+      <c r="C74">
+        <v>5</v>
+      </c>
+      <c r="D74">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75">
+        <v>20</v>
+      </c>
+      <c r="C75">
+        <v>1</v>
+      </c>
+      <c r="D75">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76">
+        <v>20</v>
+      </c>
+      <c r="C76">
+        <v>5</v>
+      </c>
+      <c r="D76">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77">
+        <v>20</v>
+      </c>
+      <c r="C77">
+        <v>3</v>
+      </c>
+      <c r="D77">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78">
+        <v>20</v>
+      </c>
+      <c r="C78">
+        <v>3</v>
+      </c>
+      <c r="D78">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79">
+        <v>21</v>
+      </c>
+      <c r="C79">
+        <v>4</v>
+      </c>
+      <c r="D79">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80">
+        <v>21</v>
+      </c>
+      <c r="C80">
+        <v>3</v>
+      </c>
+      <c r="D80">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81">
+        <v>21</v>
+      </c>
+      <c r="C81">
+        <v>5</v>
+      </c>
+      <c r="D81">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82">
+        <v>22</v>
+      </c>
+      <c r="C82">
+        <v>2</v>
+      </c>
+      <c r="D82">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83">
+        <v>22</v>
+      </c>
+      <c r="C83">
+        <v>1</v>
+      </c>
+      <c r="D83">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84">
+        <v>22</v>
+      </c>
+      <c r="C84">
+        <v>3</v>
+      </c>
+      <c r="D84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85">
+        <v>22</v>
+      </c>
+      <c r="C85">
+        <v>1</v>
+      </c>
+      <c r="D85">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86">
+        <v>23</v>
+      </c>
+      <c r="C86">
+        <v>2</v>
+      </c>
+      <c r="D86">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87">
+        <v>23</v>
+      </c>
+      <c r="C87">
+        <v>3</v>
+      </c>
+      <c r="D87">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88">
+        <v>23</v>
+      </c>
+      <c r="C88">
+        <v>3</v>
+      </c>
+      <c r="D88">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89">
+        <v>24</v>
+      </c>
+      <c r="C89">
+        <v>4</v>
+      </c>
+      <c r="D89">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>89</v>
+      </c>
+      <c r="B90">
+        <v>24</v>
+      </c>
+      <c r="C90">
+        <v>5</v>
+      </c>
+      <c r="D90">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91">
+        <v>24</v>
+      </c>
+      <c r="C91">
+        <v>5</v>
+      </c>
+      <c r="D91">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92">
+        <v>25</v>
+      </c>
+      <c r="C92">
+        <v>5</v>
+      </c>
+      <c r="D92">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93">
+        <v>25</v>
+      </c>
+      <c r="C93">
+        <v>5</v>
+      </c>
+      <c r="D93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="B94">
+        <v>25</v>
+      </c>
+      <c r="C94">
+        <v>4</v>
+      </c>
+      <c r="D94">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95">
+        <v>25</v>
+      </c>
+      <c r="C95">
+        <v>1</v>
+      </c>
+      <c r="D95">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96">
+        <v>26</v>
+      </c>
+      <c r="C96">
+        <v>2</v>
+      </c>
+      <c r="D96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97">
+        <v>26</v>
+      </c>
+      <c r="C97">
+        <v>2</v>
+      </c>
+      <c r="D97">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98">
+        <v>26</v>
+      </c>
+      <c r="C98">
+        <v>1</v>
+      </c>
+      <c r="D98">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99">
+        <v>26</v>
+      </c>
+      <c r="C99">
+        <v>1</v>
+      </c>
+      <c r="D99">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100">
+        <v>26</v>
+      </c>
+      <c r="C100">
+        <v>1</v>
+      </c>
+      <c r="D100">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>100</v>
+      </c>
+      <c r="B101">
+        <v>27</v>
+      </c>
+      <c r="C101">
+        <v>1</v>
+      </c>
+      <c r="D101">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>101</v>
+      </c>
+      <c r="B102">
+        <v>27</v>
+      </c>
+      <c r="C102">
+        <v>5</v>
+      </c>
+      <c r="D102">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>102</v>
+      </c>
+      <c r="B103">
+        <v>27</v>
+      </c>
+      <c r="C103">
+        <v>5</v>
+      </c>
+      <c r="D103">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>103</v>
+      </c>
+      <c r="B104">
+        <v>27</v>
+      </c>
+      <c r="C104">
+        <v>4</v>
+      </c>
+      <c r="D104">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>104</v>
+      </c>
+      <c r="B105">
+        <v>27</v>
+      </c>
+      <c r="C105">
+        <v>4</v>
+      </c>
+      <c r="D105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>105</v>
+      </c>
+      <c r="B106">
+        <v>28</v>
+      </c>
+      <c r="C106">
+        <v>5</v>
+      </c>
+      <c r="D106">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>106</v>
+      </c>
+      <c r="B107">
+        <v>28</v>
+      </c>
+      <c r="C107">
+        <v>4</v>
+      </c>
+      <c r="D107">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>107</v>
+      </c>
+      <c r="B108">
+        <v>28</v>
+      </c>
+      <c r="C108">
+        <v>5</v>
+      </c>
+      <c r="D108">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>108</v>
+      </c>
+      <c r="B109">
+        <v>28</v>
+      </c>
+      <c r="C109">
+        <v>2</v>
+      </c>
+      <c r="D109">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>109</v>
+      </c>
+      <c r="B110">
+        <v>28</v>
+      </c>
+      <c r="C110">
+        <v>4</v>
+      </c>
+      <c r="D110">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>110</v>
+      </c>
+      <c r="B111">
+        <v>29</v>
+      </c>
+      <c r="C111">
+        <v>3</v>
+      </c>
+      <c r="D111">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>111</v>
+      </c>
+      <c r="B112">
+        <v>29</v>
+      </c>
+      <c r="C112">
+        <v>4</v>
+      </c>
+      <c r="D112">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>112</v>
+      </c>
+      <c r="B113">
+        <v>29</v>
+      </c>
+      <c r="C113">
+        <v>5</v>
+      </c>
+      <c r="D113">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>113</v>
+      </c>
+      <c r="B114">
+        <v>30</v>
+      </c>
+      <c r="C114">
+        <v>4</v>
+      </c>
+      <c r="D114">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>114</v>
+      </c>
+      <c r="B115">
+        <v>30</v>
+      </c>
+      <c r="C115">
+        <v>3</v>
+      </c>
+      <c r="D115">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>115</v>
+      </c>
+      <c r="B116">
+        <v>30</v>
+      </c>
+      <c r="C116">
+        <v>4</v>
+      </c>
+      <c r="D116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>116</v>
+      </c>
+      <c r="B117">
+        <v>30</v>
+      </c>
+      <c r="C117">
+        <v>5</v>
+      </c>
+      <c r="D117">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>117</v>
+      </c>
+      <c r="B118">
+        <v>31</v>
+      </c>
+      <c r="C118">
+        <v>3</v>
+      </c>
+      <c r="D118">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>118</v>
+      </c>
+      <c r="B119">
+        <v>31</v>
+      </c>
+      <c r="C119">
+        <v>5</v>
+      </c>
+      <c r="D119">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>119</v>
+      </c>
+      <c r="B120">
+        <v>31</v>
+      </c>
+      <c r="C120">
+        <v>4</v>
+      </c>
+      <c r="D120">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>120</v>
+      </c>
+      <c r="B121">
+        <v>31</v>
+      </c>
+      <c r="C121">
+        <v>2</v>
+      </c>
+      <c r="D121">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>121</v>
+      </c>
+      <c r="B122">
+        <v>32</v>
+      </c>
+      <c r="C122">
+        <v>2</v>
+      </c>
+      <c r="D122">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>122</v>
+      </c>
+      <c r="B123">
+        <v>32</v>
+      </c>
+      <c r="C123">
+        <v>5</v>
+      </c>
+      <c r="D123">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>123</v>
+      </c>
+      <c r="B124">
+        <v>32</v>
+      </c>
+      <c r="C124">
+        <v>5</v>
+      </c>
+      <c r="D124">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>124</v>
+      </c>
+      <c r="B125">
+        <v>32</v>
+      </c>
+      <c r="C125">
+        <v>3</v>
+      </c>
+      <c r="D125">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>125</v>
+      </c>
+      <c r="B126">
+        <v>33</v>
+      </c>
+      <c r="C126">
+        <v>5</v>
+      </c>
+      <c r="D126">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>126</v>
+      </c>
+      <c r="B127">
+        <v>33</v>
+      </c>
+      <c r="C127">
+        <v>1</v>
+      </c>
+      <c r="D127">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>127</v>
+      </c>
+      <c r="B128">
+        <v>33</v>
+      </c>
+      <c r="C128">
+        <v>4</v>
+      </c>
+      <c r="D128">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>128</v>
+      </c>
+      <c r="B129">
+        <v>34</v>
+      </c>
+      <c r="C129">
+        <v>1</v>
+      </c>
+      <c r="D129">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>129</v>
+      </c>
+      <c r="B130">
+        <v>34</v>
+      </c>
+      <c r="C130">
+        <v>1</v>
+      </c>
+      <c r="D130">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>130</v>
+      </c>
+      <c r="B131">
+        <v>34</v>
+      </c>
+      <c r="C131">
+        <v>3</v>
+      </c>
+      <c r="D131">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>131</v>
+      </c>
+      <c r="B132">
+        <v>34</v>
+      </c>
+      <c r="C132">
+        <v>2</v>
+      </c>
+      <c r="D132">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>132</v>
+      </c>
+      <c r="B133">
+        <v>35</v>
+      </c>
+      <c r="C133">
+        <v>3</v>
+      </c>
+      <c r="D133">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>133</v>
+      </c>
+      <c r="B134">
+        <v>35</v>
+      </c>
+      <c r="C134">
+        <v>4</v>
+      </c>
+      <c r="D134">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>134</v>
+      </c>
+      <c r="B135">
+        <v>35</v>
+      </c>
+      <c r="C135">
+        <v>1</v>
+      </c>
+      <c r="D135">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>135</v>
+      </c>
+      <c r="B136">
+        <v>35</v>
+      </c>
+      <c r="C136">
+        <v>2</v>
+      </c>
+      <c r="D136">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>136</v>
+      </c>
+      <c r="B137">
+        <v>35</v>
+      </c>
+      <c r="C137">
+        <v>5</v>
+      </c>
+      <c r="D137">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>137</v>
+      </c>
+      <c r="B138">
+        <v>36</v>
+      </c>
+      <c r="C138">
+        <v>1</v>
+      </c>
+      <c r="D138">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>138</v>
+      </c>
+      <c r="B139">
+        <v>36</v>
+      </c>
+      <c r="C139">
+        <v>1</v>
+      </c>
+      <c r="D139">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>139</v>
+      </c>
+      <c r="B140">
+        <v>36</v>
+      </c>
+      <c r="C140">
+        <v>2</v>
+      </c>
+      <c r="D140">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>140</v>
+      </c>
+      <c r="B141">
+        <v>37</v>
+      </c>
+      <c r="C141">
+        <v>5</v>
+      </c>
+      <c r="D141">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>141</v>
+      </c>
+      <c r="B142">
+        <v>37</v>
+      </c>
+      <c r="C142">
+        <v>3</v>
+      </c>
+      <c r="D142">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>142</v>
+      </c>
+      <c r="B143">
+        <v>37</v>
+      </c>
+      <c r="C143">
+        <v>3</v>
+      </c>
+      <c r="D143">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>143</v>
+      </c>
+      <c r="B144">
+        <v>37</v>
+      </c>
+      <c r="C144">
+        <v>1</v>
+      </c>
+      <c r="D144">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>144</v>
+      </c>
+      <c r="B145">
+        <v>38</v>
+      </c>
+      <c r="C145">
+        <v>1</v>
+      </c>
+      <c r="D145">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>145</v>
+      </c>
+      <c r="B146">
+        <v>38</v>
+      </c>
+      <c r="C146">
+        <v>5</v>
+      </c>
+      <c r="D146">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>146</v>
+      </c>
+      <c r="B147">
+        <v>38</v>
+      </c>
+      <c r="C147">
+        <v>4</v>
+      </c>
+      <c r="D147">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>147</v>
+      </c>
+      <c r="B148">
+        <v>38</v>
+      </c>
+      <c r="C148">
+        <v>3</v>
+      </c>
+      <c r="D148">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>148</v>
+      </c>
+      <c r="B149">
+        <v>39</v>
+      </c>
+      <c r="C149">
+        <v>3</v>
+      </c>
+      <c r="D149">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>149</v>
+      </c>
+      <c r="B150">
+        <v>39</v>
+      </c>
+      <c r="C150">
+        <v>4</v>
+      </c>
+      <c r="D150">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>150</v>
+      </c>
+      <c r="B151">
+        <v>39</v>
+      </c>
+      <c r="C151">
+        <v>4</v>
+      </c>
+      <c r="D151">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -896,7 +3212,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>

</xml_diff>